<commit_message>
suporte à estabelecimentos(não somente matriz) na geração da folha
</commit_message>
<xml_diff>
--- a/data/api/empresas.xlsx
+++ b/data/api/empresas.xlsx
@@ -1833,7 +1833,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1887,12 +1887,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1966,7 +1960,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2004,10 +1998,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2138,17 +2128,17 @@
   </sheetPr>
   <dimension ref="A1:AE123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G123" activeCellId="0" sqref="G123"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13"/>
@@ -12958,7 +12948,7 @@
       <c r="B118" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="C118" s="10" t="s">
+      <c r="C118" s="1" t="s">
         <v>577</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -12967,15 +12957,15 @@
       <c r="E118" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G118" s="10" t="s">
+      <c r="G118" s="1" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="10" t="s">
+      <c r="B119" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="C119" s="10" t="s">
+      <c r="C119" s="1" t="s">
         <v>581</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -12984,7 +12974,7 @@
       <c r="E119" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G119" s="10" t="s">
+      <c r="G119" s="1" t="s">
         <v>583</v>
       </c>
     </row>
@@ -12992,7 +12982,7 @@
       <c r="B120" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="C120" s="10" t="s">
+      <c r="C120" s="1" t="s">
         <v>585</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -13001,7 +12991,7 @@
       <c r="E120" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G120" s="10" t="s">
+      <c r="G120" s="1" t="s">
         <v>587</v>
       </c>
     </row>
@@ -13052,7 +13042,7 @@
       <c r="E123" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G123" s="10" t="s">
+      <c r="G123" s="1" t="s">
         <v>599</v>
       </c>
     </row>

</xml_diff>